<commit_message>
Add fx order, default values, empty in elements
</commit_message>
<xml_diff>
--- a/py_fx_tools_dss/IMEX_to_DSS/xlsx_DSS_xlsx/Examples/13NodeIEEE/xlsx_files/BBDD_DSS_13nodeIEEE.xlsx
+++ b/py_fx_tools_dss/IMEX_to_DSS/xlsx_DSS_xlsx/Examples/13NodeIEEE/xlsx_files/BBDD_DSS_13nodeIEEE.xlsx
@@ -638,18 +638,10 @@
       </c>
       <c r="R2" t="inlineStr"/>
       <c r="S2" t="inlineStr"/>
-      <c r="T2" t="n">
-        <v>0.01805</v>
-      </c>
-      <c r="U2" t="n">
-        <v>0.155081</v>
-      </c>
-      <c r="V2" t="n">
-        <v>100</v>
-      </c>
-      <c r="W2" t="n">
-        <v>3</v>
-      </c>
+      <c r="T2" t="inlineStr"/>
+      <c r="U2" t="inlineStr"/>
+      <c r="V2" t="inlineStr"/>
+      <c r="W2" t="inlineStr"/>
       <c r="X2" t="inlineStr"/>
       <c r="Y2" t="inlineStr"/>
       <c r="Z2" t="n">
@@ -711,18 +703,10 @@
       </c>
       <c r="R3" t="inlineStr"/>
       <c r="S3" t="inlineStr"/>
-      <c r="T3" t="n">
-        <v>0.01805</v>
-      </c>
-      <c r="U3" t="n">
-        <v>0.155081</v>
-      </c>
-      <c r="V3" t="n">
-        <v>100</v>
-      </c>
-      <c r="W3" t="n">
-        <v>3</v>
-      </c>
+      <c r="T3" t="inlineStr"/>
+      <c r="U3" t="inlineStr"/>
+      <c r="V3" t="inlineStr"/>
+      <c r="W3" t="inlineStr"/>
       <c r="X3" t="inlineStr"/>
       <c r="Y3" t="inlineStr"/>
       <c r="Z3" t="n">
@@ -784,18 +768,10 @@
       </c>
       <c r="R4" t="inlineStr"/>
       <c r="S4" t="inlineStr"/>
-      <c r="T4" t="n">
-        <v>0.01805</v>
-      </c>
-      <c r="U4" t="n">
-        <v>0.155081</v>
-      </c>
-      <c r="V4" t="n">
-        <v>100</v>
-      </c>
-      <c r="W4" t="n">
-        <v>3</v>
-      </c>
+      <c r="T4" t="inlineStr"/>
+      <c r="U4" t="inlineStr"/>
+      <c r="V4" t="inlineStr"/>
+      <c r="W4" t="inlineStr"/>
       <c r="X4" t="inlineStr"/>
       <c r="Y4" t="inlineStr"/>
       <c r="Z4" t="n">
@@ -857,18 +833,10 @@
       </c>
       <c r="R5" t="inlineStr"/>
       <c r="S5" t="inlineStr"/>
-      <c r="T5" t="n">
-        <v>0.01805</v>
-      </c>
-      <c r="U5" t="n">
-        <v>0.155081</v>
-      </c>
-      <c r="V5" t="n">
-        <v>100</v>
-      </c>
-      <c r="W5" t="n">
-        <v>3</v>
-      </c>
+      <c r="T5" t="inlineStr"/>
+      <c r="U5" t="inlineStr"/>
+      <c r="V5" t="inlineStr"/>
+      <c r="W5" t="inlineStr"/>
       <c r="X5" t="inlineStr"/>
       <c r="Y5" t="inlineStr"/>
       <c r="Z5" t="n">
@@ -930,18 +898,10 @@
       </c>
       <c r="R6" t="inlineStr"/>
       <c r="S6" t="inlineStr"/>
-      <c r="T6" t="n">
-        <v>0.01805</v>
-      </c>
-      <c r="U6" t="n">
-        <v>0.155081</v>
-      </c>
-      <c r="V6" t="n">
-        <v>100</v>
-      </c>
-      <c r="W6" t="n">
-        <v>3</v>
-      </c>
+      <c r="T6" t="inlineStr"/>
+      <c r="U6" t="inlineStr"/>
+      <c r="V6" t="inlineStr"/>
+      <c r="W6" t="inlineStr"/>
       <c r="X6" t="inlineStr"/>
       <c r="Y6" t="inlineStr"/>
       <c r="Z6" t="n">
@@ -1003,18 +963,10 @@
       </c>
       <c r="R7" t="inlineStr"/>
       <c r="S7" t="inlineStr"/>
-      <c r="T7" t="n">
-        <v>0.01805</v>
-      </c>
-      <c r="U7" t="n">
-        <v>0.155081</v>
-      </c>
-      <c r="V7" t="n">
-        <v>100</v>
-      </c>
-      <c r="W7" t="n">
-        <v>3</v>
-      </c>
+      <c r="T7" t="inlineStr"/>
+      <c r="U7" t="inlineStr"/>
+      <c r="V7" t="inlineStr"/>
+      <c r="W7" t="inlineStr"/>
       <c r="X7" t="inlineStr"/>
       <c r="Y7" t="inlineStr"/>
       <c r="Z7" t="n">
@@ -1076,18 +1028,10 @@
       </c>
       <c r="R8" t="inlineStr"/>
       <c r="S8" t="inlineStr"/>
-      <c r="T8" t="n">
-        <v>0.01805</v>
-      </c>
-      <c r="U8" t="n">
-        <v>0.155081</v>
-      </c>
-      <c r="V8" t="n">
-        <v>100</v>
-      </c>
-      <c r="W8" t="n">
-        <v>2</v>
-      </c>
+      <c r="T8" t="inlineStr"/>
+      <c r="U8" t="inlineStr"/>
+      <c r="V8" t="inlineStr"/>
+      <c r="W8" t="inlineStr"/>
       <c r="X8" t="inlineStr"/>
       <c r="Y8" t="inlineStr"/>
       <c r="Z8" t="n">
@@ -1149,18 +1093,10 @@
       </c>
       <c r="R9" t="inlineStr"/>
       <c r="S9" t="inlineStr"/>
-      <c r="T9" t="n">
-        <v>0.01805</v>
-      </c>
-      <c r="U9" t="n">
-        <v>0.155081</v>
-      </c>
-      <c r="V9" t="n">
-        <v>100</v>
-      </c>
-      <c r="W9" t="n">
-        <v>2</v>
-      </c>
+      <c r="T9" t="inlineStr"/>
+      <c r="U9" t="inlineStr"/>
+      <c r="V9" t="inlineStr"/>
+      <c r="W9" t="inlineStr"/>
       <c r="X9" t="inlineStr"/>
       <c r="Y9" t="inlineStr"/>
       <c r="Z9" t="n">
@@ -1222,18 +1158,10 @@
       </c>
       <c r="R10" t="inlineStr"/>
       <c r="S10" t="inlineStr"/>
-      <c r="T10" t="n">
-        <v>0.01805</v>
-      </c>
-      <c r="U10" t="n">
-        <v>0.155081</v>
-      </c>
-      <c r="V10" t="n">
-        <v>100</v>
-      </c>
-      <c r="W10" t="n">
-        <v>1</v>
-      </c>
+      <c r="T10" t="inlineStr"/>
+      <c r="U10" t="inlineStr"/>
+      <c r="V10" t="inlineStr"/>
+      <c r="W10" t="inlineStr"/>
       <c r="X10" t="inlineStr"/>
       <c r="Y10" t="inlineStr"/>
       <c r="Z10" t="n">
@@ -1295,18 +1223,10 @@
       </c>
       <c r="R11" t="inlineStr"/>
       <c r="S11" t="inlineStr"/>
-      <c r="T11" t="n">
-        <v>0.01805</v>
-      </c>
-      <c r="U11" t="n">
-        <v>0.155081</v>
-      </c>
-      <c r="V11" t="n">
-        <v>100</v>
-      </c>
-      <c r="W11" t="n">
-        <v>1</v>
-      </c>
+      <c r="T11" t="inlineStr"/>
+      <c r="U11" t="inlineStr"/>
+      <c r="V11" t="inlineStr"/>
+      <c r="W11" t="inlineStr"/>
       <c r="X11" t="inlineStr"/>
       <c r="Y11" t="inlineStr"/>
       <c r="Z11" t="n">
@@ -1368,18 +1288,10 @@
       </c>
       <c r="R12" t="inlineStr"/>
       <c r="S12" t="inlineStr"/>
-      <c r="T12" t="n">
-        <v>0.01805</v>
-      </c>
-      <c r="U12" t="n">
-        <v>0.155081</v>
-      </c>
-      <c r="V12" t="n">
-        <v>100</v>
-      </c>
-      <c r="W12" t="n">
-        <v>1</v>
-      </c>
+      <c r="T12" t="inlineStr"/>
+      <c r="U12" t="inlineStr"/>
+      <c r="V12" t="inlineStr"/>
+      <c r="W12" t="inlineStr"/>
       <c r="X12" t="inlineStr"/>
       <c r="Y12" t="inlineStr"/>
       <c r="Z12" t="n">
@@ -1441,18 +1353,10 @@
       </c>
       <c r="R13" t="inlineStr"/>
       <c r="S13" t="inlineStr"/>
-      <c r="T13" t="n">
-        <v>0.01805</v>
-      </c>
-      <c r="U13" t="n">
-        <v>0.155081</v>
-      </c>
-      <c r="V13" t="n">
-        <v>100</v>
-      </c>
-      <c r="W13" t="n">
-        <v>3</v>
-      </c>
+      <c r="T13" t="inlineStr"/>
+      <c r="U13" t="inlineStr"/>
+      <c r="V13" t="inlineStr"/>
+      <c r="W13" t="inlineStr"/>
       <c r="X13" t="inlineStr"/>
       <c r="Y13" t="inlineStr"/>
       <c r="Z13" t="n">
@@ -1514,18 +1418,10 @@
       </c>
       <c r="R14" t="inlineStr"/>
       <c r="S14" t="inlineStr"/>
-      <c r="T14" t="n">
-        <v>0.01805</v>
-      </c>
-      <c r="U14" t="n">
-        <v>0.155081</v>
-      </c>
-      <c r="V14" t="n">
-        <v>100</v>
-      </c>
-      <c r="W14" t="n">
-        <v>3</v>
-      </c>
+      <c r="T14" t="inlineStr"/>
+      <c r="U14" t="inlineStr"/>
+      <c r="V14" t="inlineStr"/>
+      <c r="W14" t="inlineStr"/>
       <c r="X14" t="inlineStr"/>
       <c r="Y14" t="inlineStr"/>
       <c r="Z14" t="n">
@@ -1587,18 +1483,10 @@
       </c>
       <c r="R15" t="inlineStr"/>
       <c r="S15" t="inlineStr"/>
-      <c r="T15" t="n">
-        <v>0.01805</v>
-      </c>
-      <c r="U15" t="n">
-        <v>0.155081</v>
-      </c>
-      <c r="V15" t="n">
-        <v>100</v>
-      </c>
-      <c r="W15" t="n">
-        <v>3</v>
-      </c>
+      <c r="T15" t="inlineStr"/>
+      <c r="U15" t="inlineStr"/>
+      <c r="V15" t="inlineStr"/>
+      <c r="W15" t="inlineStr"/>
       <c r="X15" t="inlineStr"/>
       <c r="Y15" t="inlineStr"/>
       <c r="Z15" t="n">
@@ -1660,18 +1548,10 @@
       </c>
       <c r="R16" t="inlineStr"/>
       <c r="S16" t="inlineStr"/>
-      <c r="T16" t="n">
-        <v>0.01805</v>
-      </c>
-      <c r="U16" t="n">
-        <v>0.155081</v>
-      </c>
-      <c r="V16" t="n">
-        <v>100</v>
-      </c>
-      <c r="W16" t="n">
-        <v>1</v>
-      </c>
+      <c r="T16" t="inlineStr"/>
+      <c r="U16" t="inlineStr"/>
+      <c r="V16" t="inlineStr"/>
+      <c r="W16" t="inlineStr"/>
       <c r="X16" t="inlineStr"/>
       <c r="Y16" t="inlineStr"/>
       <c r="Z16" t="n">
@@ -1733,18 +1613,10 @@
       </c>
       <c r="R17" t="inlineStr"/>
       <c r="S17" t="inlineStr"/>
-      <c r="T17" t="n">
-        <v>0.01805</v>
-      </c>
-      <c r="U17" t="n">
-        <v>0.155081</v>
-      </c>
-      <c r="V17" t="n">
-        <v>100</v>
-      </c>
-      <c r="W17" t="n">
-        <v>1</v>
-      </c>
+      <c r="T17" t="inlineStr"/>
+      <c r="U17" t="inlineStr"/>
+      <c r="V17" t="inlineStr"/>
+      <c r="W17" t="inlineStr"/>
       <c r="X17" t="inlineStr"/>
       <c r="Y17" t="inlineStr"/>
       <c r="Z17" t="n">
@@ -1806,18 +1678,10 @@
       </c>
       <c r="R18" t="inlineStr"/>
       <c r="S18" t="inlineStr"/>
-      <c r="T18" t="n">
-        <v>0.01805</v>
-      </c>
-      <c r="U18" t="n">
-        <v>0.155081</v>
-      </c>
-      <c r="V18" t="n">
-        <v>100</v>
-      </c>
-      <c r="W18" t="n">
-        <v>1</v>
-      </c>
+      <c r="T18" t="inlineStr"/>
+      <c r="U18" t="inlineStr"/>
+      <c r="V18" t="inlineStr"/>
+      <c r="W18" t="inlineStr"/>
       <c r="X18" t="inlineStr"/>
       <c r="Y18" t="inlineStr"/>
       <c r="Z18" t="n">
@@ -1879,18 +1743,10 @@
       </c>
       <c r="R19" t="inlineStr"/>
       <c r="S19" t="inlineStr"/>
-      <c r="T19" t="n">
-        <v>0.01805</v>
-      </c>
-      <c r="U19" t="n">
-        <v>0.155081</v>
-      </c>
-      <c r="V19" t="n">
-        <v>100</v>
-      </c>
-      <c r="W19" t="n">
-        <v>3</v>
-      </c>
+      <c r="T19" t="inlineStr"/>
+      <c r="U19" t="inlineStr"/>
+      <c r="V19" t="inlineStr"/>
+      <c r="W19" t="inlineStr"/>
       <c r="X19" t="inlineStr"/>
       <c r="Y19" t="inlineStr"/>
       <c r="Z19" t="n">
@@ -1952,18 +1808,10 @@
       </c>
       <c r="R20" t="inlineStr"/>
       <c r="S20" t="inlineStr"/>
-      <c r="T20" t="n">
-        <v>0.01805</v>
-      </c>
-      <c r="U20" t="n">
-        <v>0.155081</v>
-      </c>
-      <c r="V20" t="n">
-        <v>100</v>
-      </c>
-      <c r="W20" t="n">
-        <v>3</v>
-      </c>
+      <c r="T20" t="inlineStr"/>
+      <c r="U20" t="inlineStr"/>
+      <c r="V20" t="inlineStr"/>
+      <c r="W20" t="inlineStr"/>
       <c r="X20" t="inlineStr"/>
       <c r="Y20" t="inlineStr"/>
       <c r="Z20" t="n">
@@ -2025,18 +1873,10 @@
       </c>
       <c r="R21" t="inlineStr"/>
       <c r="S21" t="inlineStr"/>
-      <c r="T21" t="n">
-        <v>0.01805</v>
-      </c>
-      <c r="U21" t="n">
-        <v>0.155081</v>
-      </c>
-      <c r="V21" t="n">
-        <v>100</v>
-      </c>
-      <c r="W21" t="n">
-        <v>3</v>
-      </c>
+      <c r="T21" t="inlineStr"/>
+      <c r="U21" t="inlineStr"/>
+      <c r="V21" t="inlineStr"/>
+      <c r="W21" t="inlineStr"/>
       <c r="X21" t="inlineStr"/>
       <c r="Y21" t="inlineStr"/>
       <c r="Z21" t="n">
@@ -2098,18 +1938,10 @@
       </c>
       <c r="R22" t="inlineStr"/>
       <c r="S22" t="inlineStr"/>
-      <c r="T22" t="n">
-        <v>0.01805</v>
-      </c>
-      <c r="U22" t="n">
-        <v>0.155081</v>
-      </c>
-      <c r="V22" t="n">
-        <v>100</v>
-      </c>
-      <c r="W22" t="n">
-        <v>2</v>
-      </c>
+      <c r="T22" t="inlineStr"/>
+      <c r="U22" t="inlineStr"/>
+      <c r="V22" t="inlineStr"/>
+      <c r="W22" t="inlineStr"/>
       <c r="X22" t="inlineStr"/>
       <c r="Y22" t="inlineStr"/>
       <c r="Z22" t="n">
@@ -2171,18 +2003,10 @@
       </c>
       <c r="R23" t="inlineStr"/>
       <c r="S23" t="inlineStr"/>
-      <c r="T23" t="n">
-        <v>0.01805</v>
-      </c>
-      <c r="U23" t="n">
-        <v>0.155081</v>
-      </c>
-      <c r="V23" t="n">
-        <v>100</v>
-      </c>
-      <c r="W23" t="n">
-        <v>2</v>
-      </c>
+      <c r="T23" t="inlineStr"/>
+      <c r="U23" t="inlineStr"/>
+      <c r="V23" t="inlineStr"/>
+      <c r="W23" t="inlineStr"/>
       <c r="X23" t="inlineStr"/>
       <c r="Y23" t="inlineStr"/>
       <c r="Z23" t="n">
@@ -2244,18 +2068,10 @@
       </c>
       <c r="R24" t="inlineStr"/>
       <c r="S24" t="inlineStr"/>
-      <c r="T24" t="n">
-        <v>0.01805</v>
-      </c>
-      <c r="U24" t="n">
-        <v>0.155081</v>
-      </c>
-      <c r="V24" t="n">
-        <v>100</v>
-      </c>
-      <c r="W24" t="n">
-        <v>1</v>
-      </c>
+      <c r="T24" t="inlineStr"/>
+      <c r="U24" t="inlineStr"/>
+      <c r="V24" t="inlineStr"/>
+      <c r="W24" t="inlineStr"/>
       <c r="X24" t="inlineStr"/>
       <c r="Y24" t="inlineStr"/>
       <c r="Z24" t="n">
@@ -2317,18 +2133,10 @@
       </c>
       <c r="R25" t="inlineStr"/>
       <c r="S25" t="inlineStr"/>
-      <c r="T25" t="n">
-        <v>0.01805</v>
-      </c>
-      <c r="U25" t="n">
-        <v>0.155081</v>
-      </c>
-      <c r="V25" t="n">
-        <v>100</v>
-      </c>
-      <c r="W25" t="n">
-        <v>3</v>
-      </c>
+      <c r="T25" t="inlineStr"/>
+      <c r="U25" t="inlineStr"/>
+      <c r="V25" t="inlineStr"/>
+      <c r="W25" t="inlineStr"/>
       <c r="X25" t="inlineStr"/>
       <c r="Y25" t="inlineStr"/>
       <c r="Z25" t="n">
@@ -2390,18 +2198,10 @@
       </c>
       <c r="R26" t="inlineStr"/>
       <c r="S26" t="inlineStr"/>
-      <c r="T26" t="n">
-        <v>0.01805</v>
-      </c>
-      <c r="U26" t="n">
-        <v>0.155081</v>
-      </c>
-      <c r="V26" t="n">
-        <v>100</v>
-      </c>
-      <c r="W26" t="n">
-        <v>1</v>
-      </c>
+      <c r="T26" t="inlineStr"/>
+      <c r="U26" t="inlineStr"/>
+      <c r="V26" t="inlineStr"/>
+      <c r="W26" t="inlineStr"/>
       <c r="X26" t="inlineStr"/>
       <c r="Y26" t="inlineStr"/>
       <c r="Z26" t="n">
@@ -2463,18 +2263,10 @@
       </c>
       <c r="R27" t="inlineStr"/>
       <c r="S27" t="inlineStr"/>
-      <c r="T27" t="n">
-        <v>0.01805</v>
-      </c>
-      <c r="U27" t="n">
-        <v>0.155081</v>
-      </c>
-      <c r="V27" t="n">
-        <v>100</v>
-      </c>
-      <c r="W27" t="n">
-        <v>3</v>
-      </c>
+      <c r="T27" t="inlineStr"/>
+      <c r="U27" t="inlineStr"/>
+      <c r="V27" t="inlineStr"/>
+      <c r="W27" t="inlineStr"/>
       <c r="X27" t="inlineStr"/>
       <c r="Y27" t="inlineStr"/>
       <c r="Z27" t="n">
@@ -2536,18 +2328,10 @@
       </c>
       <c r="R28" t="inlineStr"/>
       <c r="S28" t="inlineStr"/>
-      <c r="T28" t="n">
-        <v>0.01805</v>
-      </c>
-      <c r="U28" t="n">
-        <v>0.155081</v>
-      </c>
-      <c r="V28" t="n">
-        <v>100</v>
-      </c>
-      <c r="W28" t="n">
-        <v>3</v>
-      </c>
+      <c r="T28" t="inlineStr"/>
+      <c r="U28" t="inlineStr"/>
+      <c r="V28" t="inlineStr"/>
+      <c r="W28" t="inlineStr"/>
       <c r="X28" t="inlineStr"/>
       <c r="Y28" t="inlineStr"/>
       <c r="Z28" t="n">
@@ -2609,18 +2393,10 @@
       </c>
       <c r="R29" t="inlineStr"/>
       <c r="S29" t="inlineStr"/>
-      <c r="T29" t="n">
-        <v>0.01805</v>
-      </c>
-      <c r="U29" t="n">
-        <v>0.155081</v>
-      </c>
-      <c r="V29" t="n">
-        <v>100</v>
-      </c>
-      <c r="W29" t="n">
-        <v>3</v>
-      </c>
+      <c r="T29" t="inlineStr"/>
+      <c r="U29" t="inlineStr"/>
+      <c r="V29" t="inlineStr"/>
+      <c r="W29" t="inlineStr"/>
       <c r="X29" t="inlineStr"/>
       <c r="Y29" t="inlineStr"/>
       <c r="Z29" t="n">
@@ -2682,18 +2458,10 @@
       </c>
       <c r="R30" t="inlineStr"/>
       <c r="S30" t="inlineStr"/>
-      <c r="T30" t="n">
-        <v>0.01805</v>
-      </c>
-      <c r="U30" t="n">
-        <v>0.155081</v>
-      </c>
-      <c r="V30" t="n">
-        <v>100</v>
-      </c>
-      <c r="W30" t="n">
-        <v>3</v>
-      </c>
+      <c r="T30" t="inlineStr"/>
+      <c r="U30" t="inlineStr"/>
+      <c r="V30" t="inlineStr"/>
+      <c r="W30" t="inlineStr"/>
       <c r="X30" t="inlineStr"/>
       <c r="Y30" t="inlineStr"/>
       <c r="Z30" t="n">
@@ -2759,18 +2527,10 @@
       </c>
       <c r="R31" t="inlineStr"/>
       <c r="S31" t="inlineStr"/>
-      <c r="T31" t="n">
-        <v>0.01805</v>
-      </c>
-      <c r="U31" t="n">
-        <v>0.155081</v>
-      </c>
-      <c r="V31" t="n">
-        <v>100</v>
-      </c>
-      <c r="W31" t="n">
-        <v>3</v>
-      </c>
+      <c r="T31" t="inlineStr"/>
+      <c r="U31" t="inlineStr"/>
+      <c r="V31" t="inlineStr"/>
+      <c r="W31" t="inlineStr"/>
       <c r="X31" t="inlineStr"/>
       <c r="Y31" t="inlineStr"/>
       <c r="Z31" t="n">
@@ -2836,18 +2596,10 @@
       </c>
       <c r="R32" t="inlineStr"/>
       <c r="S32" t="inlineStr"/>
-      <c r="T32" t="n">
-        <v>0.01805</v>
-      </c>
-      <c r="U32" t="n">
-        <v>0.155081</v>
-      </c>
-      <c r="V32" t="n">
-        <v>100</v>
-      </c>
-      <c r="W32" t="n">
-        <v>3</v>
-      </c>
+      <c r="T32" t="inlineStr"/>
+      <c r="U32" t="inlineStr"/>
+      <c r="V32" t="inlineStr"/>
+      <c r="W32" t="inlineStr"/>
       <c r="X32" t="inlineStr"/>
       <c r="Y32" t="inlineStr"/>
       <c r="Z32" t="n">
@@ -2913,18 +2665,10 @@
       </c>
       <c r="R33" t="inlineStr"/>
       <c r="S33" t="inlineStr"/>
-      <c r="T33" t="n">
-        <v>0.01805</v>
-      </c>
-      <c r="U33" t="n">
-        <v>0.155081</v>
-      </c>
-      <c r="V33" t="n">
-        <v>100</v>
-      </c>
-      <c r="W33" t="n">
-        <v>2</v>
-      </c>
+      <c r="T33" t="inlineStr"/>
+      <c r="U33" t="inlineStr"/>
+      <c r="V33" t="inlineStr"/>
+      <c r="W33" t="inlineStr"/>
       <c r="X33" t="inlineStr"/>
       <c r="Y33" t="inlineStr"/>
       <c r="Z33" t="n">
@@ -2990,18 +2734,10 @@
       </c>
       <c r="R34" t="inlineStr"/>
       <c r="S34" t="inlineStr"/>
-      <c r="T34" t="n">
-        <v>0.01805</v>
-      </c>
-      <c r="U34" t="n">
-        <v>0.155081</v>
-      </c>
-      <c r="V34" t="n">
-        <v>100</v>
-      </c>
-      <c r="W34" t="n">
-        <v>2</v>
-      </c>
+      <c r="T34" t="inlineStr"/>
+      <c r="U34" t="inlineStr"/>
+      <c r="V34" t="inlineStr"/>
+      <c r="W34" t="inlineStr"/>
       <c r="X34" t="inlineStr"/>
       <c r="Y34" t="inlineStr"/>
       <c r="Z34" t="n">
@@ -3067,18 +2803,10 @@
       </c>
       <c r="R35" t="inlineStr"/>
       <c r="S35" t="inlineStr"/>
-      <c r="T35" t="n">
-        <v>0.01805</v>
-      </c>
-      <c r="U35" t="n">
-        <v>0.155081</v>
-      </c>
-      <c r="V35" t="n">
-        <v>100</v>
-      </c>
-      <c r="W35" t="n">
-        <v>1</v>
-      </c>
+      <c r="T35" t="inlineStr"/>
+      <c r="U35" t="inlineStr"/>
+      <c r="V35" t="inlineStr"/>
+      <c r="W35" t="inlineStr"/>
       <c r="X35" t="inlineStr"/>
       <c r="Y35" t="inlineStr"/>
       <c r="Z35" t="n">
@@ -3144,18 +2872,10 @@
       </c>
       <c r="R36" t="inlineStr"/>
       <c r="S36" t="inlineStr"/>
-      <c r="T36" t="n">
-        <v>0.01805</v>
-      </c>
-      <c r="U36" t="n">
-        <v>0.155081</v>
-      </c>
-      <c r="V36" t="n">
-        <v>100</v>
-      </c>
-      <c r="W36" t="n">
-        <v>3</v>
-      </c>
+      <c r="T36" t="inlineStr"/>
+      <c r="U36" t="inlineStr"/>
+      <c r="V36" t="inlineStr"/>
+      <c r="W36" t="inlineStr"/>
       <c r="X36" t="inlineStr"/>
       <c r="Y36" t="inlineStr"/>
       <c r="Z36" t="n">
@@ -3221,18 +2941,10 @@
       </c>
       <c r="R37" t="inlineStr"/>
       <c r="S37" t="inlineStr"/>
-      <c r="T37" t="n">
-        <v>0.01805</v>
-      </c>
-      <c r="U37" t="n">
-        <v>0.155081</v>
-      </c>
-      <c r="V37" t="n">
-        <v>100</v>
-      </c>
-      <c r="W37" t="n">
-        <v>1</v>
-      </c>
+      <c r="T37" t="inlineStr"/>
+      <c r="U37" t="inlineStr"/>
+      <c r="V37" t="inlineStr"/>
+      <c r="W37" t="inlineStr"/>
       <c r="X37" t="inlineStr"/>
       <c r="Y37" t="inlineStr"/>
       <c r="Z37" t="n">
@@ -3882,7 +3594,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>[0 |1.87639338887875E-310 2.25607960651843E-308 |8.96400112449967E-306 0 8.96388973297299E-306]</t>
+          <t>[0 |1.87639338887875E-310 2.25607960651843E-308 |9.25079138393353E-306 0 9.25065913350863E-306]</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -4027,112 +3739,112 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>npts</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>interval</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>mult</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>hour</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>mean</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>stddev</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>csvfile</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>sngfile</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>dblfile</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>action</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>qmult</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>UseActual</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Pmax</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Qmax</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>sinterval</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>minterval</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Pbase</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Qbase</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Pmult</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>PQCSVFile</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
           <t>MemoryMapping</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>PQCSVFile</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Pbase</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Pmax</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Pmult</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Qbase</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Qmax</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>UseActual</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>action</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>csvfile</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>dblfile</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>hour</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>interval</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>like</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>mean</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>minterval</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>mult</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>npts</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>qmult</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>sinterval</t>
-        </is>
-      </c>
-      <c r="V1" s="1" t="inlineStr">
-        <is>
-          <t>sngfile</t>
-        </is>
-      </c>
-      <c r="W1" s="1" t="inlineStr">
-        <is>
-          <t>stddev</t>
         </is>
       </c>
     </row>
@@ -4142,18 +3854,24 @@
           <t>default</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F2" t="inlineStr">
+      <c r="B2" t="n">
+        <v>24</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="inlineStr">
         <is>
           <t>[0.677 0.6256 0.6087 0.5833 0.58028 0.6025 0.657 0.7477 0.832 0.88 0.94 0.989 0.985 0.98 0.9898 0.999 1 0.958 0.936 0.913 0.876 0.876 0.828 0.756]</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="n">
+        <v>0.8258283333333341</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.15309160814381</v>
+      </c>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
@@ -4165,27 +3883,21 @@
       </c>
       <c r="O2" t="inlineStr"/>
       <c r="P2" t="n">
-        <v>0.8258283333333341</v>
+        <v>3600</v>
       </c>
       <c r="Q2" t="n">
         <v>60</v>
       </c>
-      <c r="R2" t="inlineStr">
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr"/>
+      <c r="T2" t="inlineStr">
         <is>
           <t>[0.677 0.6256 0.6087 0.5833 0.58028 0.6025 0.657 0.7477 0.832 0.88 0.94 0.989 0.985 0.98 0.9898 0.999 1 0.958 0.936 0.913 0.876 0.876 0.828 0.756]</t>
         </is>
       </c>
-      <c r="S2" t="n">
-        <v>24</v>
-      </c>
-      <c r="T2" t="inlineStr"/>
-      <c r="U2" t="n">
-        <v>3600</v>
-      </c>
+      <c r="U2" t="inlineStr"/>
       <c r="V2" t="inlineStr"/>
-      <c r="W2" t="n">
-        <v>0.15309160814381</v>
-      </c>
+      <c r="W2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4214,37 +3926,37 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>npts</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>year</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>mult</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>csvfile</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>sngfile</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>dblfile</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>like</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>mult</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>npts</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>sngfile</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>year</t>
         </is>
       </c>
     </row>
@@ -4254,23 +3966,23 @@
           <t>default</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr">
+      <c r="B2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>[1 20]</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
         <is>
           <t>[1.025 1.025]</t>
         </is>
       </c>
-      <c r="F2" t="n">
-        <v>2</v>
-      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>[1 20]</t>
-        </is>
-      </c>
+      <c r="H2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -6316,177 +6028,177 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>bus1</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>basekv</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>pu</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>angle</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>frequency</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>phases</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>MVAsc3</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>MVAsc1</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>x1r1</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>x0r0</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Isc3</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Isc1</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>R1</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>X1</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>R0</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>X0</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>ScanType</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Sequence</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>bus2</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Z1</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Z0</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Z2</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>puZ1</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>puZ0</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>puZ2</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>baseMVA</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>Yearly</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
           <t>Daily</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>Duty</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Isc1</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Isc3</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>MVAsc1</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>MVAsc3</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>Model</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>R0</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>R1</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>ScanType</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Sequence</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>X0</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>X1</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>Yearly</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>Z0</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>Z1</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>Z2</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>angle</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>baseMVA</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>puZideal</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>spectrum</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>basefreq</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
-        <is>
-          <t>basekv</t>
-        </is>
-      </c>
-      <c r="W1" s="1" t="inlineStr">
-        <is>
-          <t>bus1</t>
-        </is>
-      </c>
-      <c r="X1" s="1" t="inlineStr">
-        <is>
-          <t>bus2</t>
-        </is>
-      </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>enabled</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
-        <is>
-          <t>frequency</t>
-        </is>
-      </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>like</t>
-        </is>
-      </c>
-      <c r="AB1" s="1" t="inlineStr">
-        <is>
-          <t>phases</t>
-        </is>
-      </c>
-      <c r="AC1" s="1" t="inlineStr">
-        <is>
-          <t>pu</t>
-        </is>
-      </c>
-      <c r="AD1" s="1" t="inlineStr">
-        <is>
-          <t>puZ0</t>
-        </is>
-      </c>
-      <c r="AE1" s="1" t="inlineStr">
-        <is>
-          <t>puZ1</t>
-        </is>
-      </c>
-      <c r="AF1" s="1" t="inlineStr">
-        <is>
-          <t>puZ2</t>
-        </is>
-      </c>
-      <c r="AG1" s="1" t="inlineStr">
-        <is>
-          <t>puZideal</t>
-        </is>
-      </c>
-      <c r="AH1" s="1" t="inlineStr">
-        <is>
-          <t>spectrum</t>
-        </is>
-      </c>
-      <c r="AI1" s="1" t="inlineStr">
-        <is>
-          <t>x0r0</t>
-        </is>
-      </c>
-      <c r="AJ1" s="1" t="inlineStr">
-        <is>
-          <t>x1r1</t>
         </is>
       </c>
     </row>
@@ -6496,131 +6208,131 @@
           <t>source</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>sourcebus</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>115</v>
+      </c>
       <c r="D2" t="n">
+        <v>1.0001</v>
+      </c>
+      <c r="E2" t="n">
+        <v>30</v>
+      </c>
+      <c r="F2" t="n">
+        <v>60</v>
+      </c>
+      <c r="G2" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2" t="n">
+        <v>20000</v>
+      </c>
+      <c r="I2" t="n">
+        <v>21000</v>
+      </c>
+      <c r="J2" t="n">
+        <v>4</v>
+      </c>
+      <c r="K2" t="n">
+        <v>3</v>
+      </c>
+      <c r="L2" t="n">
+        <v>100408.742467761</v>
+      </c>
+      <c r="M2" t="n">
         <v>105429.179591149</v>
       </c>
-      <c r="E2" t="n">
-        <v>100408.742467761</v>
-      </c>
-      <c r="F2" t="n">
-        <v>21000</v>
-      </c>
-      <c r="G2" t="n">
-        <v>20000</v>
-      </c>
-      <c r="H2" t="inlineStr">
+      <c r="N2" t="n">
+        <v>0.160376682055275</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0.641506728221101</v>
+      </c>
+      <c r="P2" t="n">
+        <v>0.179603583012336</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0.538810749037007</v>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>sourcebus.0.0.0</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>[0.160376682055275, 0.641506728221101]</t>
+        </is>
+      </c>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>[0.179603583012336, 0.538810749037007]</t>
+        </is>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>[0.160376682055275, 0.641506728221101]</t>
+        </is>
+      </c>
+      <c r="X2" t="inlineStr">
+        <is>
+          <t>[0.00121267812518166, 0.00485071250072666]</t>
+        </is>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>[0.0013580611191859, 0.00407418335755771]</t>
+        </is>
+      </c>
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t>[0.00121267812518166, 0.00485071250072666]</t>
+        </is>
+      </c>
+      <c r="AA2" t="n">
+        <v>100</v>
+      </c>
+      <c r="AB2" t="inlineStr"/>
+      <c r="AC2" t="inlineStr"/>
+      <c r="AD2" t="inlineStr"/>
+      <c r="AE2" t="inlineStr">
         <is>
           <t>Thevenin</t>
         </is>
       </c>
-      <c r="I2" t="n">
-        <v>0.179603583012336</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0.160376682055275</v>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>Positive</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>Positive</t>
-        </is>
-      </c>
-      <c r="M2" t="n">
-        <v>0.538810749037007</v>
-      </c>
-      <c r="N2" t="n">
-        <v>0.641506728221101</v>
-      </c>
-      <c r="O2" t="inlineStr"/>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>[0.179603583012336, 0.538810749037007]</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>[0.160376682055275, 0.641506728221101]</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>[0.160376682055275, 0.641506728221101]</t>
-        </is>
-      </c>
-      <c r="S2" t="n">
-        <v>30</v>
-      </c>
-      <c r="T2" t="n">
-        <v>100</v>
-      </c>
-      <c r="U2" t="n">
+      <c r="AF2" t="inlineStr">
+        <is>
+          <t>[1e-06, 0.001]</t>
+        </is>
+      </c>
+      <c r="AG2" t="inlineStr">
+        <is>
+          <t>defaultvsource</t>
+        </is>
+      </c>
+      <c r="AH2" t="n">
         <v>60</v>
       </c>
-      <c r="V2" t="n">
-        <v>115</v>
-      </c>
-      <c r="W2" t="inlineStr">
-        <is>
-          <t>sourcebus</t>
-        </is>
-      </c>
-      <c r="X2" t="inlineStr">
-        <is>
-          <t>sourcebus.0.0.0</t>
-        </is>
-      </c>
-      <c r="Y2" t="inlineStr">
+      <c r="AI2" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="Z2" t="n">
-        <v>60</v>
-      </c>
-      <c r="AA2" t="inlineStr"/>
-      <c r="AB2" t="n">
-        <v>3</v>
-      </c>
-      <c r="AC2" t="n">
-        <v>1.0001</v>
-      </c>
-      <c r="AD2" t="inlineStr">
-        <is>
-          <t>[0.0013580611191859, 0.00407418335755771]</t>
-        </is>
-      </c>
-      <c r="AE2" t="inlineStr">
-        <is>
-          <t>[0.00121267812518166, 0.00485071250072666]</t>
-        </is>
-      </c>
-      <c r="AF2" t="inlineStr">
-        <is>
-          <t>[0.00121267812518166, 0.00485071250072666]</t>
-        </is>
-      </c>
-      <c r="AG2" t="inlineStr">
-        <is>
-          <t>[1e-06, 0.001]</t>
-        </is>
-      </c>
-      <c r="AH2" t="inlineStr">
-        <is>
-          <t>defaultvsource</t>
-        </is>
-      </c>
-      <c r="AI2" t="n">
-        <v>3</v>
-      </c>
-      <c r="AJ2" t="n">
-        <v>4</v>
-      </c>
+      <c r="AJ2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>